<commit_message>
Word List 1 updated with pictures.
</commit_message>
<xml_diff>
--- a/res/Book1.xlsx
+++ b/res/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>introspection</t>
   </si>
@@ -96,12 +96,6 @@
     <t xml:space="preserve">attract, lure </t>
   </si>
   <si>
-    <t>alleviate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make (pain) easier to bear </t>
-  </si>
-  <si>
     <t>adorn</t>
   </si>
   <si>
@@ -166,6 +160,78 @@
   </si>
   <si>
     <t xml:space="preserve">a person who is attracted to foreign peoples cultures </t>
+  </si>
+  <si>
+    <t>introspection.jpg</t>
+  </si>
+  <si>
+    <t>philanthropist.jpg</t>
+  </si>
+  <si>
+    <t>antidote.jpg</t>
+  </si>
+  <si>
+    <t>strive.jpg</t>
+  </si>
+  <si>
+    <t>ambidextrous.jpg</t>
+  </si>
+  <si>
+    <t>retrospective.jpg</t>
+  </si>
+  <si>
+    <t>precursors.jpg</t>
+  </si>
+  <si>
+    <t>introvert.jpg</t>
+  </si>
+  <si>
+    <t>gerontocracy.jpg</t>
+  </si>
+  <si>
+    <t>ambiguous.jpg</t>
+  </si>
+  <si>
+    <t>braggart.jpg</t>
+  </si>
+  <si>
+    <t>aggravate.jpg</t>
+  </si>
+  <si>
+    <t>entice.jpg</t>
+  </si>
+  <si>
+    <t>adorn.jpg</t>
+  </si>
+  <si>
+    <t>equilibrium.jpg</t>
+  </si>
+  <si>
+    <t>abhor.jpg</t>
+  </si>
+  <si>
+    <t>connote.jpg</t>
+  </si>
+  <si>
+    <t>endeavor.jpg</t>
+  </si>
+  <si>
+    <t>agile.jpg</t>
+  </si>
+  <si>
+    <t>renovate.jpg</t>
+  </si>
+  <si>
+    <t>curriculum.jpg</t>
+  </si>
+  <si>
+    <t>malevolent.jpg</t>
+  </si>
+  <si>
+    <t>amalgamate.jpg</t>
+  </si>
+  <si>
+    <t>xenophile.jpg</t>
   </si>
 </sst>
 </file>
@@ -518,212 +584,281 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52" customWidth="1"/>
+    <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>49</v>
+      <c r="C24" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>